<commit_message>
feat: testing multipart file
</commit_message>
<xml_diff>
--- a/src/main/resources/Patologias.xlsx
+++ b/src/main/resources/Patologias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backend\estudos\excel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A5EAEC-8CA9-46B4-9423-CBE29E09CD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8C6478-0EB5-4AF6-AC68-380031D37BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{230ED5A7-69BD-42FB-92F5-39CDABB523CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{230ED5A7-69BD-42FB-92F5-39CDABB523CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Patologia</t>
   </si>
@@ -56,19 +56,22 @@
     <t>Elétrica</t>
   </si>
   <si>
-    <t>Ambiental</t>
-  </si>
-  <si>
-    <t>Teste</t>
-  </si>
-  <si>
-    <t>sdgsg</t>
-  </si>
-  <si>
-    <t>hguuyo</t>
-  </si>
-  <si>
-    <t>gfdbdd</t>
+    <t>Esquadria fora de prumo</t>
+  </si>
+  <si>
+    <t>Esquadrias</t>
+  </si>
+  <si>
+    <t>Instalações aparentes</t>
+  </si>
+  <si>
+    <t>Pintura irregular</t>
+  </si>
+  <si>
+    <t>Conservação</t>
+  </si>
+  <si>
+    <t>Resíduos</t>
   </si>
 </sst>
 </file>
@@ -470,38 +473,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>